<commit_message>
-Pricing fixes -Quote Sheet Changes
</commit_message>
<xml_diff>
--- a/ogserver/src/data/templates/quote-template.xlsx
+++ b/ogserver/src/data/templates/quote-template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7455" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Quote" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>No 1502, 1st Floor, 19th Main, Sector 1, HSR Layout</t>
   </si>
   <si>
-    <t>Kapture E-ID</t>
-  </si>
-  <si>
     <t>Bangalore 560 102, India</t>
   </si>
   <si>
@@ -478,6 +475,9 @@
   </si>
   <si>
     <t>Estimated Cost after Discount(A + B - C) -</t>
+  </si>
+  <si>
+    <t>CRM Id</t>
   </si>
 </sst>
 </file>
@@ -1422,6 +1422,93 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1463,93 +1550,6 @@
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="22" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="27" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="25" fillId="0" borderId="28" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="27" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -1895,8 +1895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView view="pageBreakPreview" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,11 +1913,11 @@
     <row r="1" spans="1:5" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="93" t="s">
+      <c r="C1" s="122" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="93"/>
-      <c r="E1" s="94"/>
+      <c r="D1" s="122"/>
+      <c r="E1" s="123"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
@@ -1934,7 +1934,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1944,44 +1944,44 @@
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="10" t="s">
-        <v>3</v>
+        <v>72</v>
       </c>
       <c r="E4" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="7"/>
@@ -1989,20 +1989,20 @@
     </row>
     <row r="8" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" s="4"/>
       <c r="E8" s="14"/>
     </row>
     <row r="9" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="17"/>
@@ -2010,92 +2010,92 @@
     </row>
     <row r="10" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="82" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="83" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="7"/>
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="96"/>
+      <c r="A11" s="124" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="125"/>
       <c r="C11" s="18"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="100"/>
+      <c r="D11" s="128"/>
+      <c r="E11" s="129"/>
     </row>
     <row r="12" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="97"/>
-      <c r="B12" s="98"/>
+      <c r="A12" s="126"/>
+      <c r="B12" s="127"/>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
       <c r="E12" s="21"/>
     </row>
     <row r="13" spans="1:5" s="51" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="50" t="s">
+      <c r="C13" s="130" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="101" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="102"/>
-      <c r="E13" s="103"/>
+      <c r="D13" s="131"/>
+      <c r="E13" s="132"/>
     </row>
     <row r="14" spans="1:5" s="51" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B14" s="85" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="115" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="110" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="111"/>
-      <c r="E14" s="112"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="117"/>
     </row>
     <row r="15" spans="1:5" s="51" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
-        <v>66</v>
-      </c>
-      <c r="B15" s="105"/>
-      <c r="C15" s="105"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
+      <c r="A15" s="133" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="134"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="134"/>
+      <c r="E15" s="135"/>
     </row>
     <row r="16" spans="1:5" s="51" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="53" t="s">
+      <c r="C16" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="53" t="s">
+      <c r="D16" s="54" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="54" t="s">
+      <c r="E16" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="55" t="s">
+    </row>
+    <row r="17" spans="1:12" s="51" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="112" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" s="51" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="108"/>
-      <c r="C17" s="108"/>
-      <c r="D17" s="109"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="113"/>
+      <c r="D17" s="114"/>
       <c r="E17" s="56" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F17" s="57"/>
       <c r="G17" s="58"/>
@@ -2111,10 +2111,10 @@
     </row>
     <row r="19" spans="1:12" s="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" s="61" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="62"/>
       <c r="D19" s="62"/>
@@ -2124,10 +2124,10 @@
     </row>
     <row r="20" spans="1:12" s="65" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="73" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B20" s="61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="62"/>
       <c r="D20" s="62"/>
@@ -2146,10 +2146,10 @@
     </row>
     <row r="22" spans="1:12" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="73" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="61" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="62"/>
       <c r="D22" s="80"/>
@@ -2178,10 +2178,10 @@
     </row>
     <row r="24" spans="1:12" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="73" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="61" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C24" s="71"/>
       <c r="D24" s="72"/>
@@ -2210,10 +2210,10 @@
     </row>
     <row r="26" spans="1:12" s="65" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="73" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B26" s="61" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C26" s="62"/>
       <c r="D26" s="80"/>
@@ -2241,14 +2241,14 @@
       <c r="L27" s="68"/>
     </row>
     <row r="28" spans="1:12" s="31" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="107" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="108"/>
-      <c r="C28" s="108"/>
-      <c r="D28" s="109"/>
+      <c r="A28" s="112" t="s">
+        <v>20</v>
+      </c>
+      <c r="B28" s="113"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="114"/>
       <c r="E28" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F28" s="33"/>
       <c r="G28"/>
@@ -2266,14 +2266,14 @@
       <c r="E29" s="30"/>
     </row>
     <row r="30" spans="1:12" s="31" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="107" t="s">
-        <v>22</v>
-      </c>
-      <c r="B30" s="108"/>
-      <c r="C30" s="108"/>
-      <c r="D30" s="109"/>
+      <c r="A30" s="112" t="s">
+        <v>21</v>
+      </c>
+      <c r="B30" s="113"/>
+      <c r="C30" s="113"/>
+      <c r="D30" s="114"/>
       <c r="E30" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F30" s="33"/>
       <c r="G30"/>
@@ -2284,14 +2284,14 @@
       <c r="L30"/>
     </row>
     <row r="31" spans="1:12" s="92" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="115" t="s">
-        <v>71</v>
-      </c>
-      <c r="B31" s="116"/>
-      <c r="C31" s="116"/>
-      <c r="D31" s="116"/>
+      <c r="A31" s="120" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="121"/>
+      <c r="C31" s="121"/>
+      <c r="D31" s="121"/>
       <c r="E31" s="89" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F31" s="90"/>
       <c r="G31" s="91"/>
@@ -2302,14 +2302,14 @@
       <c r="L31" s="91"/>
     </row>
     <row r="32" spans="1:12" s="31" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="107" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="108"/>
-      <c r="C32" s="108"/>
-      <c r="D32" s="108"/>
+      <c r="A32" s="112" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="113"/>
+      <c r="C32" s="113"/>
+      <c r="D32" s="113"/>
       <c r="E32" s="88" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F32" s="33"/>
       <c r="G32"/>
@@ -2328,14 +2328,14 @@
     </row>
     <row r="34" spans="1:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="84" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="113" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34" s="113"/>
-      <c r="D34" s="113"/>
-      <c r="E34" s="114"/>
+        <v>39</v>
+      </c>
+      <c r="B34" s="118" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="118"/>
+      <c r="D34" s="118"/>
+      <c r="E34" s="119"/>
     </row>
     <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
@@ -2345,141 +2345,141 @@
       <c r="E35" s="38"/>
     </row>
     <row r="36" spans="1:5" s="39" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="130" t="s">
+      <c r="A36" s="99" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="100"/>
+      <c r="C36" s="100"/>
+      <c r="D36" s="100"/>
+      <c r="E36" s="101"/>
+    </row>
+    <row r="37" spans="1:5" s="39" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="102" t="s">
         <v>23</v>
       </c>
-      <c r="B36" s="131"/>
-      <c r="C36" s="131"/>
-      <c r="D36" s="131"/>
-      <c r="E36" s="132"/>
-    </row>
-    <row r="37" spans="1:5" s="39" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="133" t="s">
+      <c r="B37" s="103"/>
+      <c r="C37" s="103"/>
+      <c r="D37" s="103"/>
+      <c r="E37" s="104"/>
+    </row>
+    <row r="38" spans="1:5" s="39" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="93" t="s">
         <v>24</v>
       </c>
-      <c r="B37" s="134"/>
-      <c r="C37" s="134"/>
-      <c r="D37" s="134"/>
-      <c r="E37" s="135"/>
-    </row>
-    <row r="38" spans="1:5" s="39" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="127" t="s">
+      <c r="B38" s="94"/>
+      <c r="C38" s="94"/>
+      <c r="D38" s="94"/>
+      <c r="E38" s="95"/>
+    </row>
+    <row r="39" spans="1:5" s="39" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="93" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="128"/>
-      <c r="C38" s="128"/>
-      <c r="D38" s="128"/>
-      <c r="E38" s="129"/>
-    </row>
-    <row r="39" spans="1:5" s="39" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="127" t="s">
+      <c r="B39" s="94"/>
+      <c r="C39" s="94"/>
+      <c r="D39" s="94"/>
+      <c r="E39" s="95"/>
+    </row>
+    <row r="40" spans="1:5" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="93" t="s">
         <v>26</v>
       </c>
-      <c r="B39" s="128"/>
-      <c r="C39" s="128"/>
-      <c r="D39" s="128"/>
-      <c r="E39" s="129"/>
-    </row>
-    <row r="40" spans="1:5" s="39" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="127" t="s">
+      <c r="B40" s="94"/>
+      <c r="C40" s="94"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="95"/>
+    </row>
+    <row r="41" spans="1:5" s="39" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="93" t="s">
         <v>27</v>
       </c>
-      <c r="B40" s="128"/>
-      <c r="C40" s="128"/>
-      <c r="D40" s="128"/>
-      <c r="E40" s="129"/>
-    </row>
-    <row r="41" spans="1:5" s="39" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="127" t="s">
+      <c r="B41" s="94"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="94"/>
+      <c r="E41" s="95"/>
+    </row>
+    <row r="42" spans="1:5" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="93" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="128"/>
-      <c r="C41" s="128"/>
-      <c r="D41" s="128"/>
-      <c r="E41" s="129"/>
-    </row>
-    <row r="42" spans="1:5" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="127" t="s">
+      <c r="B42" s="40" t="s">
         <v>29</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>30</v>
       </c>
       <c r="C42" s="40"/>
       <c r="D42" s="40"/>
       <c r="E42" s="41"/>
     </row>
     <row r="43" spans="1:5" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="127"/>
+      <c r="A43" s="93"/>
       <c r="B43" s="40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
       <c r="E43" s="41"/>
     </row>
     <row r="44" spans="1:5" s="39" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="127"/>
+      <c r="A44" s="93"/>
       <c r="B44" s="42" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C44" s="40"/>
       <c r="D44" s="40"/>
       <c r="E44" s="41"/>
     </row>
     <row r="45" spans="1:5" s="39" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="124" t="s">
+      <c r="A45" s="96" t="s">
+        <v>32</v>
+      </c>
+      <c r="B45" s="97"/>
+      <c r="C45" s="97"/>
+      <c r="D45" s="97"/>
+      <c r="E45" s="98"/>
+    </row>
+    <row r="46" spans="1:5" s="39" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="96" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="125"/>
-      <c r="C45" s="125"/>
-      <c r="D45" s="125"/>
-      <c r="E45" s="126"/>
-    </row>
-    <row r="46" spans="1:5" s="39" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="124" t="s">
+      <c r="B46" s="97"/>
+      <c r="C46" s="97"/>
+      <c r="D46" s="97"/>
+      <c r="E46" s="98"/>
+    </row>
+    <row r="47" spans="1:5" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="93" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="125"/>
-      <c r="C46" s="125"/>
-      <c r="D46" s="125"/>
-      <c r="E46" s="126"/>
-    </row>
-    <row r="47" spans="1:5" s="39" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="127" t="s">
+      <c r="B47" s="94"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="94"/>
+      <c r="E47" s="95"/>
+    </row>
+    <row r="48" spans="1:5" s="39" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="93" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="128"/>
-      <c r="C47" s="128"/>
-      <c r="D47" s="128"/>
-      <c r="E47" s="129"/>
-    </row>
-    <row r="48" spans="1:5" s="39" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="127" t="s">
+      <c r="B48" s="94"/>
+      <c r="C48" s="94"/>
+      <c r="D48" s="94"/>
+      <c r="E48" s="95"/>
+    </row>
+    <row r="49" spans="1:5" s="39" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="B48" s="128"/>
-      <c r="C48" s="128"/>
-      <c r="D48" s="128"/>
-      <c r="E48" s="129"/>
-    </row>
-    <row r="49" spans="1:5" s="39" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="119" t="s">
+      <c r="B49" s="108"/>
+      <c r="C49" s="108"/>
+      <c r="D49" s="108"/>
+      <c r="E49" s="109"/>
+    </row>
+    <row r="50" spans="1:5" s="39" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="120"/>
-      <c r="C49" s="120"/>
-      <c r="D49" s="120"/>
-      <c r="E49" s="121"/>
-    </row>
-    <row r="50" spans="1:5" s="39" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="119" t="s">
-        <v>38</v>
-      </c>
-      <c r="B50" s="120"/>
-      <c r="C50" s="120"/>
-      <c r="D50" s="120"/>
-      <c r="E50" s="121"/>
+      <c r="B50" s="108"/>
+      <c r="C50" s="108"/>
+      <c r="D50" s="108"/>
+      <c r="E50" s="109"/>
     </row>
     <row r="51" spans="1:5" s="39" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="43"/>
@@ -2489,19 +2489,38 @@
       <c r="E51" s="45"/>
     </row>
     <row r="52" spans="1:5" s="39" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="122" t="s">
-        <v>39</v>
-      </c>
-      <c r="B52" s="123"/>
+      <c r="A52" s="110" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="111"/>
       <c r="C52" s="46"/>
-      <c r="D52" s="117" t="s">
-        <v>42</v>
-      </c>
-      <c r="E52" s="118"/>
+      <c r="D52" s="105" t="s">
+        <v>41</v>
+      </c>
+      <c r="E52" s="106"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/7JB1jPPyAHyYl9rtZA9l2HZuQmqCTekZ5XaNCrrGOnJQVFoomp55fGvq+Jdl/YPuxAZx7QIagol29NuJkVqtA==" saltValue="qVFB4YnPArTZdgOcUV4AUw==" spinCount="100000" sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="27">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="A11:B12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="B34:E34"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="A49:E49"/>
+    <mergeCell ref="A50:E50"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="A48:E48"/>
     <mergeCell ref="A41:E41"/>
     <mergeCell ref="A42:A44"/>
     <mergeCell ref="A45:E45"/>
@@ -2510,25 +2529,6 @@
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A39:E39"/>
     <mergeCell ref="A40:E40"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="A49:E49"/>
-    <mergeCell ref="A50:E50"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="A48:E48"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="B34:E34"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="A11:B12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="A15:E15"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1" display="mailto:shubha.t@mygubbi.com"/>
@@ -2544,7 +2544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>